<commit_message>
Parameters are done for some time.
</commit_message>
<xml_diff>
--- a/server/data/database.xlsx
+++ b/server/data/database.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="174">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -274,15 +274,21 @@
     <t xml:space="preserve">waterProtection</t>
   </si>
   <si>
+    <t xml:space="preserve">IP00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет защиты от твердых предметов.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет защиты от воды.</t>
+  </si>
+  <si>
     <t xml:space="preserve">IP01</t>
   </si>
   <si>
     <t xml:space="preserve">Защита от предметов диаметром более 50 мм.</t>
   </si>
   <si>
-    <t xml:space="preserve">Нет защиты от воды.</t>
-  </si>
-  <si>
     <t xml:space="preserve">IP02</t>
   </si>
   <si>
@@ -310,7 +316,7 @@
     <t xml:space="preserve">IP06</t>
   </si>
   <si>
-    <t xml:space="preserve">Защита от сильных струй воды</t>
+    <t xml:space="preserve">Защита от сильных струй воды (например, на палубе корабля).</t>
   </si>
   <si>
     <t xml:space="preserve">IP07</t>
@@ -331,6 +337,9 @@
     <t xml:space="preserve">Защита от высокотемпературной струи воды под высоким давлением.</t>
   </si>
   <si>
+    <t xml:space="preserve">IP10</t>
+  </si>
+  <si>
     <t xml:space="preserve">IP11</t>
   </si>
   <si>
@@ -373,12 +382,15 @@
     <t xml:space="preserve">Защита от высокотемпературной струи воды.</t>
   </si>
   <si>
+    <t xml:space="preserve">IP20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Защита от предметов диаметром более 12,5 мм.</t>
+  </si>
+  <si>
     <t xml:space="preserve">IP21</t>
   </si>
   <si>
-    <t xml:space="preserve">Защита от предметов диаметром более 12,5 мм.</t>
-  </si>
-  <si>
     <t xml:space="preserve">IP22</t>
   </si>
   <si>
@@ -403,12 +415,15 @@
     <t xml:space="preserve">IP29</t>
   </si>
   <si>
+    <t xml:space="preserve">IP30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Защита от предметов диаметром более 2,5 мм.</t>
+  </si>
+  <si>
     <t xml:space="preserve">IP31</t>
   </si>
   <si>
-    <t xml:space="preserve">Защита от предметов диаметром более 2,5 мм.</t>
-  </si>
-  <si>
     <t xml:space="preserve">IP32</t>
   </si>
   <si>
@@ -433,12 +448,15 @@
     <t xml:space="preserve">IP39</t>
   </si>
   <si>
+    <t xml:space="preserve">IP40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Защита от предметов диаметром более 1 мм.</t>
+  </si>
+  <si>
     <t xml:space="preserve">IP41</t>
   </si>
   <si>
-    <t xml:space="preserve">Защита от предметов диаметром более 1 мм.</t>
-  </si>
-  <si>
     <t xml:space="preserve">IP42</t>
   </si>
   <si>
@@ -463,12 +481,15 @@
     <t xml:space="preserve">IP49</t>
   </si>
   <si>
+    <t xml:space="preserve">IP50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Частичная защита от пыли.</t>
+  </si>
+  <si>
     <t xml:space="preserve">IP51</t>
   </si>
   <si>
-    <t xml:space="preserve">Частичная защита от пыли.</t>
-  </si>
-  <si>
     <t xml:space="preserve">IP52</t>
   </si>
   <si>
@@ -493,10 +514,13 @@
     <t xml:space="preserve">IP59</t>
   </si>
   <si>
+    <t xml:space="preserve">IP60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Полная защита от пыли.</t>
+  </si>
+  <si>
     <t xml:space="preserve">IP61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Полная защита от пыли.</t>
   </si>
   <si>
     <t xml:space="preserve">IP62</t>
@@ -738,7 +762,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2228,17 +2252,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="68.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="68.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,10 +2292,10 @@
         <v>86</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2279,7 +2303,7 @@
         <v>88</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>89</v>
@@ -2290,7 +2314,7 @@
         <v>90</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>91</v>
@@ -2301,7 +2325,7 @@
         <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>93</v>
@@ -2312,7 +2336,7 @@
         <v>94</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>95</v>
@@ -2323,7 +2347,7 @@
         <v>96</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>97</v>
@@ -2334,7 +2358,7 @@
         <v>98</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>99</v>
@@ -2345,7 +2369,7 @@
         <v>100</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>101</v>
@@ -2356,7 +2380,7 @@
         <v>102</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>103</v>
@@ -2367,10 +2391,10 @@
         <v>104</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2378,43 +2402,43 @@
         <v>105</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2422,54 +2446,54 @@
         <v>110</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2477,87 +2501,87 @@
         <v>119</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,10 +2589,10 @@
         <v>128</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2576,10 +2600,10 @@
         <v>129</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,76 +2611,76 @@
         <v>130</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="C33" s="3" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,10 +2688,10 @@
         <v>138</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2675,10 +2699,10 @@
         <v>139</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2686,10 +2710,10 @@
         <v>140</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2697,65 +2721,65 @@
         <v>141</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="C43" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2763,10 +2787,10 @@
         <v>148</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2774,10 +2798,10 @@
         <v>149</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2785,10 +2809,10 @@
         <v>150</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2796,10 +2820,10 @@
         <v>151</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2807,54 +2831,54 @@
         <v>152</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="C53" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2862,10 +2886,10 @@
         <v>158</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2873,10 +2897,10 @@
         <v>159</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2884,10 +2908,10 @@
         <v>160</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2895,10 +2919,10 @@
         <v>161</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2906,10 +2930,10 @@
         <v>162</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,32 +2941,109 @@
         <v>163</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="C63" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C64" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>